<commit_message>
latest datstes plus tex revised
</commit_message>
<xml_diff>
--- a/Lancelotti2015impr/datasets/Jandhala_dataset.xlsx
+++ b/Lancelotti2015impr/datasets/Jandhala_dataset.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="0" windowWidth="34120" windowHeight="15940" tabRatio="837" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="700" yWindow="0" windowWidth="34120" windowHeight="15940" tabRatio="837" firstSheet="7" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Extractions" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1945" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1967" uniqueCount="284">
   <si>
     <t>ID</t>
   </si>
@@ -888,16 +888,22 @@
   <si>
     <t>**** Some tracheid and LC are burnt</t>
   </si>
+  <si>
+    <t>Graminoids_leaf/culm</t>
+  </si>
+  <si>
+    <t>Graminoids_inflorescence</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="172" formatCode="0.0"/>
-    <numFmt numFmtId="173" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -947,11 +953,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
@@ -983,10 +984,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -998,7 +1013,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1017,7 +1032,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1034,19 +1049,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1139,28 +1168,879 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:areaChart>
-        <c:grouping val="percentStacked"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>summary!$D$1</c:f>
+              <c:f>summary!$D$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Herbaceous_leaf/culm</c:v>
+                  <c:v>Graminoids_leaf/culm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="66CCFF"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>summary!$A$17:$B$26</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="10"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Outer_control</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Inner_control</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Fireplace</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Outer_control</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Inner_control</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Fireplace</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Outer_control</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Inner_control</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Fireplace</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Veranda</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Inside_left</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Inside_right</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Floor</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$D$17:$D$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.634304207119741</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.073115003808073</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.90342679127726</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.177033492822966</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.03669008587041</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.14893617021277</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.975267930750206</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.615384615384614</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.87085514834206</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$E$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Graminoids_inflorescence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0"/>
+                  <c:y val="0.0406551707028096"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0"/>
+                  <c:y val="0.0383965501082093"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>summary!$A$17:$B$26</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="10"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Outer_control</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Inner_control</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Fireplace</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Outer_control</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Inner_control</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Fireplace</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Outer_control</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Inner_control</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Fireplace</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Veranda</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Inside_left</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Inside_right</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Floor</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$E$17:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.779935275080906</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.351104341203351</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.672897196261682</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.189792663476874</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.810304449648712</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.64741641337386</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.978565539983512</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.884615384615385</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.143258213825025</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$G$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Woody_species</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.26402043954906E-17"/>
+                  <c:y val="0.0338793089190081"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>summary!$A$17:$B$26</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="10"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Outer_control</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Inner_control</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Fireplace</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Outer_control</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Inner_control</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Fireplace</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Outer_control</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Inner_control</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Fireplace</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Veranda</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Inside_left</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Inside_right</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Floor</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$G$17:$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.26537216828479</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.056359482102057</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.246105919003115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.75438596491228</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.327088212334114</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.319043693322341</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.32051282051282</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.864709006753168</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$H$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Indet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0"/>
+                  <c:y val="0.00903448237840209"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.52804087909813E-17"/>
+                  <c:y val="0.00903448237840218"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.52804087909813E-17"/>
+                  <c:y val="0.00677586178380163"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0"/>
+                  <c:y val="0.00903448237840218"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.05608175819626E-17"/>
+                  <c:y val="0.00677586178380163"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0"/>
+                  <c:y val="0.0112931029730027"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0"/>
+                  <c:y val="0.00677586178380155"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0"/>
+                  <c:y val="0.00677586178380155"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0"/>
+                  <c:y val="0.00903448237840218"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0"/>
+                  <c:y val="0.0135517235676033"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>summary!$A$17:$B$26</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="10"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Outer_control</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Inner_control</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Fireplace</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Outer_control</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Inner_control</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Fireplace</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Outer_control</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Inner_control</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Fireplace</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Veranda</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Inside_left</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Inside_right</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Floor</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$H$17:$H$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.074433656957929</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.397562833206398</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.29595015576324</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.379585326953748</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.401249024199843</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.382978723404255</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.677658697444353</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.57692307692308</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.389255633963123</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2115358792"/>
+        <c:axId val="2115361880"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2115358792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2115361880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2115361880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>%</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2115358792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
               <c:f>summary!$A$2:$B$11</c:f>
@@ -1214,63 +2094,80 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>summary!$D$2:$D$11</c:f>
+              <c:f>summary!$I$17:$I$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>20.5</c:v>
+                  <c:v>55.51664890004362</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.5</c:v>
+                  <c:v>55.414882385289</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>35.0</c:v>
+                <c:pt idx="2">
+                  <c:v>54.08719556114549</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.5</c:v>
+                  <c:v>57.09202005843797</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.75</c:v>
+                  <c:v>57.30390792154653</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>63.0</c:v>
+                <c:pt idx="5">
+                  <c:v>60.28553160701966</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.5</c:v>
+                  <c:v>56.91844911358828</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30.25</c:v>
+                  <c:v>58.29250428345344</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>30.0</c:v>
+                <c:pt idx="8">
+                  <c:v>61.07920446085357</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40.38690476190476</c:v>
+                  <c:v>57.45402512311731</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>summary!$E$1</c:f>
+              <c:f>summary!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Herbaceous_inflorescence</c:v>
+                  <c:v>Wood</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="0080FF"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
             </a:solidFill>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
               <c:f>summary!$A$2:$B$11</c:f>
@@ -1324,267 +2221,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>summary!$E$2:$E$11</c:f>
+              <c:f>summary!$J$17:$J$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5.5</c:v>
+                  <c:v>44.48335109995637</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.0</c:v>
+                  <c:v>44.585117614711</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>15.0</c:v>
+                <c:pt idx="2">
+                  <c:v>45.91280443885451</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.0</c:v>
+                  <c:v>42.90797994156203</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.0</c:v>
+                  <c:v>42.69609207845347</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>12.0</c:v>
+                <c:pt idx="5">
+                  <c:v>39.71446839298033</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>43.08155088641171</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.0</c:v>
+                  <c:v>41.70749571654655</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>9.0</c:v>
+                <c:pt idx="8">
+                  <c:v>38.92079553914643</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.863095238095237</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>summary!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Woody_species</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="0000FF"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw dist="35921" dir="2700000" algn="br">
-                <a:srgbClr val="000000"/>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>summary!$A$2:$B$11</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Outer_control</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Inner_control</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Fireplace</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Outer_control</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Inner_control</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Fireplace</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Outer_control</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Inner_control</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Fireplace</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Veranda</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Inside_left</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Inside_right</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Floor</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>summary!$G$2:$G$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.75</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.25</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.851190476190476</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>summary!$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Indet</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004080"/>
-            </a:solidFill>
-          </c:spPr>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>summary!$A$2:$B$11</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Outer_control</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Inner_control</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Fireplace</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Outer_control</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Inner_control</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Fireplace</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Outer_control</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Inner_control</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Fireplace</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Veranda</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Inside_left</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Inside_right</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Floor</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>summary!$H$2:$H$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20.5</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20.25</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>33.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>16.91071428571428</c:v>
+                  <c:v>42.54597487688267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1598,345 +2267,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2126785384"/>
-        <c:axId val="2079433080"/>
-      </c:areaChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="2107791624"/>
+        <c:axId val="2107774136"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="2126785384"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2079433080"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2079433080"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126785384"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:noFill/>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:areaChart>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>summary!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Dung</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="bg2">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>summary!$A$2:$B$11</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Outer_control</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Inner_control</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Fireplace</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Outer_control</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Inner_control</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Fireplace</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Outer_control</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Inner_control</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Fireplace</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Veranda</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Inside_left</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Inside_right</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Floor</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>summary!$I$2:$I$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1234.285</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1100.915</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2455.51</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1156.73</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1291.6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>716.59</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1128.69</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1114.2175</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>804.01</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1208.672261904762</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>summary!$J$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Wood</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>summary!$A$2:$B$11</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Outer_control</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Inner_control</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Fireplace</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Outer_control</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Inner_control</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Fireplace</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Outer_control</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Inner_control</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Fireplace</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Veranda</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Inside_left</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Inside_right</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Floor</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>summary!$J$2:$J$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0" formatCode="0.00">
-                  <c:v>988.985</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>885.7625</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0.00">
-                  <c:v>2084.4</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.00">
-                  <c:v>869.35</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.00">
-                  <c:v>962.3475</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.00">
-                  <c:v>472.07</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.00">
-                  <c:v>854.3050000000001</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.00">
-                  <c:v>797.2075</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.00">
-                  <c:v>512.33</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="0.00">
-                  <c:v>895.0485119047619</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2125672824"/>
-        <c:axId val="2125669800"/>
-      </c:areaChart>
-      <c:catAx>
-        <c:axId val="2125672824"/>
+        <c:axId val="2107791624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1947,7 +2283,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-5400000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1956,7 +2292,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125669800"/>
+        <c:crossAx val="2107774136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1964,19 +2300,38 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125669800"/>
+        <c:axId val="2107774136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>%</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125672824"/>
+        <c:crossAx val="2107791624"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2022,7 +2377,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="131" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -22065,15 +22420,18 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
@@ -22084,10 +22442,10 @@
         <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>90</v>
+        <v>282</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>91</v>
+        <v>283</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>92</v>
@@ -22105,8 +22463,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" s="33" t="s">
         <v>89</v>
       </c>
       <c r="B2" t="s">
@@ -22136,9 +22494,17 @@
       <c r="J2" s="23">
         <v>988.98500000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="31"/>
+      <c r="K2" s="23">
+        <f>SUM(D2:H2)</f>
+        <v>309</v>
+      </c>
+      <c r="L2" s="23">
+        <f>SUM(I2:J2)</f>
+        <v>2223.27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="33"/>
       <c r="B3" t="s">
         <v>85</v>
       </c>
@@ -22166,9 +22532,17 @@
       <c r="J3" s="1">
         <v>885.76250000000005</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="31"/>
+      <c r="K3" s="23">
+        <f t="shared" ref="K3:K11" si="0">SUM(D3:H3)</f>
+        <v>328.25</v>
+      </c>
+      <c r="L3" s="23">
+        <f t="shared" ref="L3:L11" si="1">SUM(I3:J3)</f>
+        <v>1986.6775</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="33"/>
       <c r="B4" t="s">
         <v>82</v>
       </c>
@@ -22196,9 +22570,17 @@
       <c r="J4" s="23">
         <v>2084.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="31" t="s">
+      <c r="K4" s="23">
+        <f t="shared" si="0"/>
+        <v>321</v>
+      </c>
+      <c r="L4" s="23">
+        <f t="shared" si="1"/>
+        <v>4539.91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="33" t="s">
         <v>88</v>
       </c>
       <c r="B5" t="s">
@@ -22228,9 +22610,17 @@
       <c r="J5" s="23">
         <v>869.35</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="31"/>
+      <c r="K5" s="23">
+        <f t="shared" si="0"/>
+        <v>313.5</v>
+      </c>
+      <c r="L5" s="23">
+        <f t="shared" si="1"/>
+        <v>2026.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="33"/>
       <c r="B6" t="s">
         <v>85</v>
       </c>
@@ -22258,9 +22648,17 @@
       <c r="J6" s="23">
         <v>962.34749999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="31"/>
+      <c r="K6" s="23">
+        <f t="shared" si="0"/>
+        <v>320.25</v>
+      </c>
+      <c r="L6" s="23">
+        <f t="shared" si="1"/>
+        <v>2253.9475000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="33"/>
       <c r="B7" t="s">
         <v>82</v>
       </c>
@@ -22288,9 +22686,17 @@
       <c r="J7" s="23">
         <v>472.07</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="31" t="s">
+      <c r="K7" s="23">
+        <f t="shared" si="0"/>
+        <v>329</v>
+      </c>
+      <c r="L7" s="23">
+        <f t="shared" si="1"/>
+        <v>1188.6600000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="33" t="s">
         <v>83</v>
       </c>
       <c r="B8" t="s">
@@ -22320,9 +22726,17 @@
       <c r="J8" s="23">
         <v>854.30500000000006</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="31"/>
+      <c r="K8" s="23">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="L8" s="23">
+        <f t="shared" si="1"/>
+        <v>1982.9950000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="33"/>
       <c r="B9" t="s">
         <v>85</v>
       </c>
@@ -22350,9 +22764,17 @@
       <c r="J9" s="23">
         <v>797.20749999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="31"/>
+      <c r="K9" s="23">
+        <f t="shared" si="0"/>
+        <v>303.25</v>
+      </c>
+      <c r="L9" s="23">
+        <f t="shared" si="1"/>
+        <v>1911.425</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="33"/>
       <c r="B10" t="s">
         <v>82</v>
       </c>
@@ -22380,8 +22802,16 @@
       <c r="J10" s="23">
         <v>512.33000000000004</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="23">
+        <f t="shared" si="0"/>
+        <v>312</v>
+      </c>
+      <c r="L10" s="23">
+        <f t="shared" si="1"/>
+        <v>1316.3400000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>195</v>
       </c>
@@ -22409,12 +22839,455 @@
       <c r="J11" s="23">
         <v>895.04851190476188</v>
       </c>
+      <c r="K11" s="23">
+        <f t="shared" si="0"/>
+        <v>313.78571428571428</v>
+      </c>
+      <c r="L11" s="23">
+        <f t="shared" si="1"/>
+        <v>2103.720773809524</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="2"/>
+      <c r="B16" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="23">
+        <v>1092066.9667478744</v>
+      </c>
+      <c r="D17" s="23">
+        <f>(D2*100/$K$2)</f>
+        <v>6.6343042071197411</v>
+      </c>
+      <c r="E17" s="23">
+        <f t="shared" ref="E17:H17" si="2">(E2*100/$K$2)</f>
+        <v>1.7799352750809061</v>
+      </c>
+      <c r="F17" s="23">
+        <f t="shared" si="2"/>
+        <v>86.245954692556637</v>
+      </c>
+      <c r="G17" s="23">
+        <f t="shared" si="2"/>
+        <v>2.2653721682847898</v>
+      </c>
+      <c r="H17" s="23">
+        <f t="shared" si="2"/>
+        <v>3.0744336569579289</v>
+      </c>
+      <c r="I17" s="23">
+        <f>(I2*100)/L2</f>
+        <v>55.51664890004362</v>
+      </c>
+      <c r="J17" s="23">
+        <f>(J2*100)/L2</f>
+        <v>44.483351099956373</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="33"/>
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="23">
+        <v>883792.39571453677</v>
+      </c>
+      <c r="D18" s="23">
+        <f>(D3*100/$K3)</f>
+        <v>8.0731150038080735</v>
+      </c>
+      <c r="E18" s="23">
+        <f t="shared" ref="E18:H18" si="3">(E3*100/$K3)</f>
+        <v>3.3511043412033512</v>
+      </c>
+      <c r="F18" s="23">
+        <f t="shared" si="3"/>
+        <v>80.121858339680117</v>
+      </c>
+      <c r="G18" s="23">
+        <f t="shared" si="3"/>
+        <v>2.0563594821020565</v>
+      </c>
+      <c r="H18" s="23">
+        <f t="shared" si="3"/>
+        <v>6.3975628332063978</v>
+      </c>
+      <c r="I18" s="23">
+        <f t="shared" ref="I18:I26" si="4">(I3*100)/L3</f>
+        <v>55.414882385289005</v>
+      </c>
+      <c r="J18" s="23">
+        <f t="shared" ref="J18:J26" si="5">(J3*100)/L3</f>
+        <v>44.585117614710995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="33"/>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="23">
+        <v>966850.11022227607</v>
+      </c>
+      <c r="D19" s="23">
+        <f>(D4*100/$K4)</f>
+        <v>10.903426791277258</v>
+      </c>
+      <c r="E19" s="23">
+        <f t="shared" ref="E19:H19" si="6">(E4*100/$K4)</f>
+        <v>4.6728971962616823</v>
+      </c>
+      <c r="F19" s="23">
+        <f t="shared" si="6"/>
+        <v>77.881619937694708</v>
+      </c>
+      <c r="G19" s="23">
+        <f t="shared" si="6"/>
+        <v>1.2461059190031152</v>
+      </c>
+      <c r="H19" s="23">
+        <f t="shared" si="6"/>
+        <v>5.29595015576324</v>
+      </c>
+      <c r="I19" s="23">
+        <f t="shared" si="4"/>
+        <v>54.087195561145492</v>
+      </c>
+      <c r="J19" s="23">
+        <f t="shared" si="5"/>
+        <v>45.912804438854515</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="23">
+        <v>1148302.4919070262</v>
+      </c>
+      <c r="D20" s="23">
+        <f t="shared" ref="D20:H20" si="7">(D5*100/$K5)</f>
+        <v>7.1770334928229662</v>
+      </c>
+      <c r="E20" s="23">
+        <f t="shared" si="7"/>
+        <v>3.1897926634768741</v>
+      </c>
+      <c r="F20" s="23">
+        <f t="shared" si="7"/>
+        <v>81.499202551834131</v>
+      </c>
+      <c r="G20" s="23">
+        <f t="shared" si="7"/>
+        <v>1.7543859649122806</v>
+      </c>
+      <c r="H20" s="23">
+        <f t="shared" si="7"/>
+        <v>6.3795853269537481</v>
+      </c>
+      <c r="I20" s="23">
+        <f t="shared" si="4"/>
+        <v>57.092020058437974</v>
+      </c>
+      <c r="J20" s="23">
+        <f t="shared" si="5"/>
+        <v>42.907979941562033</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="33"/>
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="23">
+        <v>1151112.2252124967</v>
+      </c>
+      <c r="D21" s="23">
+        <f t="shared" ref="D21:H21" si="8">(D6*100/$K6)</f>
+        <v>13.036690085870413</v>
+      </c>
+      <c r="E21" s="23">
+        <f t="shared" si="8"/>
+        <v>2.810304449648712</v>
+      </c>
+      <c r="F21" s="23">
+        <f t="shared" si="8"/>
+        <v>76.42466822794691</v>
+      </c>
+      <c r="G21" s="23">
+        <f t="shared" si="8"/>
+        <v>1.3270882123341139</v>
+      </c>
+      <c r="H21" s="23">
+        <f t="shared" si="8"/>
+        <v>6.4012490241998439</v>
+      </c>
+      <c r="I21" s="23">
+        <f t="shared" si="4"/>
+        <v>57.303907921546532</v>
+      </c>
+      <c r="J21" s="23">
+        <f t="shared" si="5"/>
+        <v>42.696092078453468</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="33"/>
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="23">
+        <v>119056.57266590041</v>
+      </c>
+      <c r="D22" s="23">
+        <f t="shared" ref="D22:H22" si="9">(D7*100/$K7)</f>
+        <v>19.148936170212767</v>
+      </c>
+      <c r="E22" s="23">
+        <f t="shared" si="9"/>
+        <v>3.6474164133738602</v>
+      </c>
+      <c r="F22" s="23">
+        <f t="shared" si="9"/>
+        <v>70.820668693009125</v>
+      </c>
+      <c r="G22" s="23">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="23">
+        <f t="shared" si="9"/>
+        <v>6.3829787234042552</v>
+      </c>
+      <c r="I22" s="23">
+        <f t="shared" si="4"/>
+        <v>60.285531607019664</v>
+      </c>
+      <c r="J22" s="23">
+        <f t="shared" si="5"/>
+        <v>39.714468392980329</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="23">
+        <v>902626.35981687554</v>
+      </c>
+      <c r="D23" s="23">
+        <f t="shared" ref="D23:H23" si="10">(D8*100/$K8)</f>
+        <v>7.5</v>
+      </c>
+      <c r="E23" s="23">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="F23" s="23">
+        <f t="shared" si="10"/>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="G23" s="23">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="H23" s="23">
+        <f t="shared" si="10"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="I23" s="23">
+        <f t="shared" si="4"/>
+        <v>56.918449113588281</v>
+      </c>
+      <c r="J23" s="23">
+        <f t="shared" si="5"/>
+        <v>43.081550886411712</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="33"/>
+      <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="23">
+        <v>514262.87810057041</v>
+      </c>
+      <c r="D24" s="23">
+        <f t="shared" ref="D24:H24" si="11">(D9*100/$K9)</f>
+        <v>9.9752679307502063</v>
+      </c>
+      <c r="E24" s="23">
+        <f t="shared" si="11"/>
+        <v>1.978565539983512</v>
+      </c>
+      <c r="F24" s="23">
+        <f t="shared" si="11"/>
+        <v>80.049464138499587</v>
+      </c>
+      <c r="G24" s="23">
+        <f t="shared" si="11"/>
+        <v>1.3190436933223413</v>
+      </c>
+      <c r="H24" s="23">
+        <f t="shared" si="11"/>
+        <v>6.677658697444353</v>
+      </c>
+      <c r="I24" s="23">
+        <f t="shared" si="4"/>
+        <v>58.292504283453447</v>
+      </c>
+      <c r="J24" s="23">
+        <f t="shared" si="5"/>
+        <v>41.707495716546553</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="33"/>
+      <c r="B25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="23">
+        <v>213991.26946089594</v>
+      </c>
+      <c r="D25" s="23">
+        <f t="shared" ref="D25:H26" si="12">(D10*100/$K10)</f>
+        <v>9.615384615384615</v>
+      </c>
+      <c r="E25" s="23">
+        <f t="shared" si="12"/>
+        <v>2.8846153846153846</v>
+      </c>
+      <c r="F25" s="23">
+        <f t="shared" si="12"/>
+        <v>76.602564102564102</v>
+      </c>
+      <c r="G25" s="23">
+        <f t="shared" si="12"/>
+        <v>0.32051282051282054</v>
+      </c>
+      <c r="H25" s="23">
+        <f t="shared" si="12"/>
+        <v>10.576923076923077</v>
+      </c>
+      <c r="I25" s="23">
+        <f t="shared" si="4"/>
+        <v>61.079204460853575</v>
+      </c>
+      <c r="J25" s="23">
+        <f t="shared" si="5"/>
+        <v>38.920795539146425</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>195</v>
+      </c>
+      <c r="C26" s="23">
+        <v>2981254.5473371679</v>
+      </c>
+      <c r="D26" s="23">
+        <f t="shared" si="12"/>
+        <v>12.870855148342059</v>
+      </c>
+      <c r="E26" s="23">
+        <f t="shared" si="12"/>
+        <v>3.1432582138250247</v>
+      </c>
+      <c r="F26" s="23">
+        <f t="shared" si="12"/>
+        <v>76.731921997116615</v>
+      </c>
+      <c r="G26" s="23">
+        <f t="shared" si="12"/>
+        <v>1.864709006753168</v>
+      </c>
+      <c r="H26" s="23">
+        <f t="shared" si="12"/>
+        <v>5.3892556339631232</v>
+      </c>
+      <c r="I26" s="23">
+        <f t="shared" si="4"/>
+        <v>57.454025123117312</v>
+      </c>
+      <c r="J26" s="23">
+        <f t="shared" si="5"/>
+        <v>42.545974876882674</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A23:A25"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -22662,7 +23535,7 @@
       </c>
     </row>
     <row r="3" spans="1:55">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="31" t="s">
         <v>205</v>
       </c>
       <c r="B3" t="s">
@@ -22826,7 +23699,7 @@
       </c>
     </row>
     <row r="4" spans="1:55">
-      <c r="A4" s="33"/>
+      <c r="A4" s="31"/>
       <c r="B4" t="s">
         <v>207</v>
       </c>
@@ -22988,7 +23861,7 @@
       </c>
     </row>
     <row r="5" spans="1:55">
-      <c r="A5" s="33"/>
+      <c r="A5" s="31"/>
       <c r="B5" t="s">
         <v>208</v>
       </c>
@@ -23111,7 +23984,7 @@
       </c>
     </row>
     <row r="6" spans="1:55">
-      <c r="A6" s="33"/>
+      <c r="A6" s="31"/>
       <c r="B6" t="s">
         <v>209</v>
       </c>
@@ -23213,7 +24086,7 @@
       </c>
     </row>
     <row r="7" spans="1:55">
-      <c r="A7" s="33"/>
+      <c r="A7" s="31"/>
       <c r="B7" t="s">
         <v>210</v>
       </c>
@@ -23303,7 +24176,7 @@
       </c>
     </row>
     <row r="8" spans="1:55">
-      <c r="A8" s="33"/>
+      <c r="A8" s="31"/>
       <c r="B8" t="s">
         <v>211</v>
       </c>
@@ -23617,7 +24490,7 @@
       </c>
     </row>
     <row r="10" spans="1:55">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="31" t="s">
         <v>212</v>
       </c>
       <c r="B10" t="s">
@@ -23781,7 +24654,7 @@
       </c>
     </row>
     <row r="11" spans="1:55">
-      <c r="A11" s="33"/>
+      <c r="A11" s="31"/>
       <c r="B11" t="s">
         <v>214</v>
       </c>
@@ -23940,7 +24813,7 @@
       </c>
     </row>
     <row r="12" spans="1:55">
-      <c r="A12" s="33"/>
+      <c r="A12" s="31"/>
       <c r="B12" t="s">
         <v>215</v>
       </c>
@@ -24102,7 +24975,7 @@
       </c>
     </row>
     <row r="13" spans="1:55">
-      <c r="A13" s="33"/>
+      <c r="A13" s="31"/>
       <c r="B13" t="s">
         <v>216</v>
       </c>
@@ -24222,7 +25095,7 @@
       </c>
     </row>
     <row r="14" spans="1:55">
-      <c r="A14" s="33"/>
+      <c r="A14" s="31"/>
       <c r="B14" t="s">
         <v>217</v>
       </c>
@@ -24342,7 +25215,7 @@
       </c>
     </row>
     <row r="15" spans="1:55">
-      <c r="A15" s="33"/>
+      <c r="A15" s="31"/>
       <c r="B15" t="s">
         <v>218</v>
       </c>
@@ -24447,7 +25320,7 @@
       </c>
     </row>
     <row r="16" spans="1:55">
-      <c r="A16" s="33"/>
+      <c r="A16" s="31"/>
       <c r="B16" t="s">
         <v>219</v>
       </c>
@@ -24609,7 +25482,7 @@
       </c>
     </row>
     <row r="17" spans="1:55">
-      <c r="A17" s="33"/>
+      <c r="A17" s="31"/>
       <c r="B17" t="s">
         <v>64</v>
       </c>
@@ -24771,7 +25644,7 @@
       </c>
     </row>
     <row r="18" spans="1:55">
-      <c r="A18" s="33"/>
+      <c r="A18" s="31"/>
       <c r="B18" t="s">
         <v>65</v>
       </c>
@@ -24930,7 +25803,7 @@
       </c>
     </row>
     <row r="19" spans="1:55">
-      <c r="A19" s="33"/>
+      <c r="A19" s="31"/>
       <c r="B19" t="s">
         <v>66</v>
       </c>
@@ -25038,7 +25911,7 @@
       </c>
     </row>
     <row r="20" spans="1:55">
-      <c r="A20" s="33"/>
+      <c r="A20" s="31"/>
       <c r="B20" t="s">
         <v>67</v>
       </c>
@@ -25200,7 +26073,7 @@
       </c>
     </row>
     <row r="21" spans="1:55">
-      <c r="A21" s="33"/>
+      <c r="A21" s="31"/>
       <c r="B21" t="s">
         <v>68</v>
       </c>
@@ -25362,7 +26235,7 @@
       </c>
     </row>
     <row r="22" spans="1:55">
-      <c r="A22" s="33"/>
+      <c r="A22" s="31"/>
       <c r="B22" t="s">
         <v>69</v>
       </c>
@@ -25524,7 +26397,7 @@
       </c>
     </row>
     <row r="23" spans="1:55">
-      <c r="A23" s="33"/>
+      <c r="A23" s="31"/>
       <c r="B23" t="s">
         <v>70</v>
       </c>
@@ -26575,7 +27448,7 @@
       </c>
     </row>
     <row r="32" spans="1:55">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="31" t="s">
         <v>78</v>
       </c>
       <c r="B32" t="s">
@@ -26736,7 +27609,7 @@
       </c>
     </row>
     <row r="33" spans="1:55">
-      <c r="A33" s="33"/>
+      <c r="A33" s="31"/>
       <c r="B33" t="s">
         <v>222</v>
       </c>
@@ -26898,7 +27771,7 @@
       </c>
     </row>
     <row r="34" spans="1:55">
-      <c r="A34" s="33"/>
+      <c r="A34" s="31"/>
       <c r="B34" t="s">
         <v>223</v>
       </c>
@@ -26994,7 +27867,7 @@
       </c>
     </row>
     <row r="35" spans="1:55">
-      <c r="A35" s="33"/>
+      <c r="A35" s="31"/>
       <c r="B35" t="s">
         <v>224</v>
       </c>
@@ -27135,7 +28008,7 @@
       </c>
     </row>
     <row r="36" spans="1:55">
-      <c r="A36" s="33"/>
+      <c r="A36" s="31"/>
       <c r="B36" t="s">
         <v>225</v>
       </c>
@@ -27222,7 +28095,7 @@
       </c>
     </row>
     <row r="37" spans="1:55">
-      <c r="A37" s="33"/>
+      <c r="A37" s="31"/>
       <c r="B37" t="s">
         <v>226</v>
       </c>
@@ -27521,7 +28394,7 @@
       </c>
     </row>
     <row r="39" spans="1:55">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="31" t="s">
         <v>227</v>
       </c>
       <c r="B39" t="s">
@@ -27664,7 +28537,7 @@
       </c>
     </row>
     <row r="40" spans="1:55">
-      <c r="A40" s="33"/>
+      <c r="A40" s="31"/>
       <c r="B40" t="s">
         <v>229</v>
       </c>
@@ -27754,7 +28627,7 @@
       </c>
     </row>
     <row r="41" spans="1:55">
-      <c r="A41" s="33"/>
+      <c r="A41" s="31"/>
       <c r="B41" t="s">
         <v>230</v>
       </c>
@@ -27850,7 +28723,7 @@
       </c>
     </row>
     <row r="42" spans="1:55">
-      <c r="A42" s="33"/>
+      <c r="A42" s="31"/>
       <c r="B42" t="s">
         <v>227</v>
       </c>
@@ -27997,7 +28870,7 @@
       </c>
     </row>
     <row r="43" spans="1:55">
-      <c r="A43" s="33"/>
+      <c r="A43" s="31"/>
       <c r="B43" t="s">
         <v>231</v>
       </c>
@@ -28266,7 +29139,7 @@
       </c>
     </row>
     <row r="45" spans="1:55">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="31" t="s">
         <v>232</v>
       </c>
       <c r="B45" t="s">
@@ -28280,7 +29153,7 @@
       </c>
     </row>
     <row r="46" spans="1:55">
-      <c r="A46" s="33"/>
+      <c r="A46" s="31"/>
       <c r="B46" t="s">
         <v>227</v>
       </c>
@@ -28289,7 +29162,7 @@
       </c>
     </row>
     <row r="47" spans="1:55">
-      <c r="A47" s="33"/>
+      <c r="A47" s="31"/>
       <c r="B47" t="s">
         <v>76</v>
       </c>
@@ -28298,7 +29171,7 @@
       </c>
     </row>
     <row r="48" spans="1:55">
-      <c r="A48" s="33"/>
+      <c r="A48" s="31"/>
       <c r="B48" t="s">
         <v>78</v>
       </c>
@@ -28307,7 +29180,7 @@
       </c>
     </row>
     <row r="49" spans="1:29">
-      <c r="A49" s="33"/>
+      <c r="A49" s="31"/>
       <c r="B49" t="s">
         <v>235</v>
       </c>
@@ -28322,7 +29195,7 @@
       </c>
     </row>
     <row r="50" spans="1:29">
-      <c r="A50" s="33"/>
+      <c r="A50" s="31"/>
       <c r="C50" t="s">
         <v>238</v>
       </c>
@@ -28331,7 +29204,7 @@
       </c>
     </row>
     <row r="51" spans="1:29">
-      <c r="A51" s="33"/>
+      <c r="A51" s="31"/>
       <c r="C51" t="s">
         <v>240</v>
       </c>
@@ -28343,7 +29216,7 @@
       </c>
     </row>
     <row r="52" spans="1:29">
-      <c r="A52" s="33"/>
+      <c r="A52" s="31"/>
       <c r="B52" t="s">
         <v>242</v>
       </c>
@@ -28358,7 +29231,7 @@
       </c>
     </row>
     <row r="53" spans="1:29">
-      <c r="A53" s="33"/>
+      <c r="A53" s="31"/>
       <c r="C53" t="s">
         <v>238</v>
       </c>
@@ -28367,7 +29240,7 @@
       </c>
     </row>
     <row r="54" spans="1:29">
-      <c r="A54" s="33"/>
+      <c r="A54" s="31"/>
       <c r="C54" t="s">
         <v>240</v>
       </c>
@@ -28376,7 +29249,7 @@
       </c>
     </row>
     <row r="55" spans="1:29">
-      <c r="A55" s="33"/>
+      <c r="A55" s="31"/>
       <c r="B55" t="s">
         <v>240</v>
       </c>
@@ -28436,7 +29309,7 @@
       </c>
     </row>
     <row r="56" spans="1:29">
-      <c r="A56" s="33"/>
+      <c r="A56" s="31"/>
       <c r="C56" t="s">
         <v>238</v>
       </c>
@@ -28478,7 +29351,7 @@
       </c>
     </row>
     <row r="57" spans="1:29">
-      <c r="A57" s="33"/>
+      <c r="A57" s="31"/>
       <c r="C57" t="s">
         <v>240</v>
       </c>
@@ -28573,7 +29446,7 @@
       </c>
     </row>
     <row r="59" spans="1:29">
-      <c r="A59" s="33" t="s">
+      <c r="A59" s="31" t="s">
         <v>255</v>
       </c>
       <c r="B59" t="s">
@@ -28626,7 +29499,7 @@
       </c>
     </row>
     <row r="60" spans="1:29">
-      <c r="A60" s="33"/>
+      <c r="A60" s="31"/>
       <c r="C60" t="s">
         <v>208</v>
       </c>
@@ -28659,7 +29532,7 @@
       </c>
     </row>
     <row r="61" spans="1:29">
-      <c r="A61" s="33"/>
+      <c r="A61" s="31"/>
       <c r="C61" t="s">
         <v>207</v>
       </c>
@@ -28695,13 +29568,13 @@
       </c>
     </row>
     <row r="62" spans="1:29">
-      <c r="A62" s="33"/>
+      <c r="A62" s="31"/>
       <c r="C62" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="63" spans="1:29">
-      <c r="A63" s="33"/>
+      <c r="A63" s="31"/>
       <c r="C63" t="s">
         <v>256</v>
       </c>
@@ -28719,7 +29592,7 @@
       </c>
     </row>
     <row r="64" spans="1:29">
-      <c r="A64" s="33"/>
+      <c r="A64" s="31"/>
       <c r="C64" t="s">
         <v>210</v>
       </c>
@@ -28731,7 +29604,7 @@
       </c>
     </row>
     <row r="65" spans="1:55">
-      <c r="A65" s="33"/>
+      <c r="A65" s="31"/>
       <c r="C65" t="s">
         <v>94</v>
       </c>
@@ -28749,7 +29622,7 @@
       </c>
     </row>
     <row r="66" spans="1:55">
-      <c r="A66" s="33"/>
+      <c r="A66" s="31"/>
       <c r="B66" t="s">
         <v>212</v>
       </c>
@@ -28770,7 +29643,7 @@
       </c>
     </row>
     <row r="67" spans="1:55">
-      <c r="A67" s="33"/>
+      <c r="A67" s="31"/>
       <c r="C67" t="s">
         <v>69</v>
       </c>
@@ -28788,13 +29661,13 @@
       </c>
     </row>
     <row r="68" spans="1:55">
-      <c r="A68" s="33"/>
+      <c r="A68" s="31"/>
       <c r="C68" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="69" spans="1:55">
-      <c r="A69" s="33"/>
+      <c r="A69" s="31"/>
       <c r="B69" t="s">
         <v>78</v>
       </c>
@@ -28806,19 +29679,19 @@
       </c>
     </row>
     <row r="70" spans="1:55">
-      <c r="A70" s="33"/>
+      <c r="A70" s="31"/>
       <c r="B70" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:55">
-      <c r="A71" s="33"/>
+      <c r="A71" s="31"/>
       <c r="B71" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:55">
-      <c r="A72" s="33"/>
+      <c r="A72" s="31"/>
       <c r="B72" t="s">
         <v>75</v>
       </c>
@@ -28827,7 +29700,7 @@
       </c>
     </row>
     <row r="73" spans="1:55">
-      <c r="A73" s="33"/>
+      <c r="A73" s="31"/>
       <c r="B73" t="s">
         <v>76</v>
       </c>
@@ -28836,7 +29709,7 @@
       </c>
     </row>
     <row r="74" spans="1:55">
-      <c r="A74" s="33"/>
+      <c r="A74" s="31"/>
       <c r="B74" t="s">
         <v>227</v>
       </c>
@@ -28845,7 +29718,7 @@
       </c>
     </row>
     <row r="75" spans="1:55">
-      <c r="A75" s="33"/>
+      <c r="A75" s="31"/>
       <c r="B75" t="s">
         <v>231</v>
       </c>
@@ -29943,7 +30816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AM2" sqref="AM2:AS2"/>
     </sheetView>
   </sheetViews>
@@ -30028,15 +30901,15 @@
       <c r="V2" s="32"/>
       <c r="W2" s="32"/>
       <c r="X2" s="32"/>
-      <c r="Y2" s="33" t="s">
+      <c r="Y2" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
       <c r="AF2" s="32" t="s">
         <v>268</v>
       </c>
@@ -30185,7 +31058,7 @@
       </c>
     </row>
     <row r="4" spans="1:45">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="31" t="s">
         <v>205</v>
       </c>
       <c r="B4" t="s">
@@ -30319,7 +31192,7 @@
       </c>
     </row>
     <row r="5" spans="1:45">
-      <c r="A5" s="33"/>
+      <c r="A5" s="31"/>
       <c r="B5" t="s">
         <v>207</v>
       </c>
@@ -30451,7 +31324,7 @@
       </c>
     </row>
     <row r="6" spans="1:45">
-      <c r="A6" s="33"/>
+      <c r="A6" s="31"/>
       <c r="B6" t="s">
         <v>208</v>
       </c>
@@ -30544,7 +31417,7 @@
       </c>
     </row>
     <row r="7" spans="1:45">
-      <c r="A7" s="33"/>
+      <c r="A7" s="31"/>
       <c r="B7" t="s">
         <v>209</v>
       </c>
@@ -30625,7 +31498,7 @@
       </c>
     </row>
     <row r="8" spans="1:45">
-      <c r="A8" s="33"/>
+      <c r="A8" s="31"/>
       <c r="B8" t="s">
         <v>211</v>
       </c>
@@ -30867,7 +31740,7 @@
       </c>
     </row>
     <row r="10" spans="1:45">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="31" t="s">
         <v>212</v>
       </c>
       <c r="B10" t="s">
@@ -31001,7 +31874,7 @@
       </c>
     </row>
     <row r="11" spans="1:45">
-      <c r="A11" s="33"/>
+      <c r="A11" s="31"/>
       <c r="B11" t="s">
         <v>214</v>
       </c>
@@ -31130,7 +32003,7 @@
       </c>
     </row>
     <row r="12" spans="1:45">
-      <c r="A12" s="33"/>
+      <c r="A12" s="31"/>
       <c r="B12" t="s">
         <v>215</v>
       </c>
@@ -31259,7 +32132,7 @@
       </c>
     </row>
     <row r="13" spans="1:45">
-      <c r="A13" s="33"/>
+      <c r="A13" s="31"/>
       <c r="B13" t="s">
         <v>216</v>
       </c>
@@ -31343,7 +32216,7 @@
       </c>
     </row>
     <row r="14" spans="1:45">
-      <c r="A14" s="33"/>
+      <c r="A14" s="31"/>
       <c r="B14" t="s">
         <v>217</v>
       </c>
@@ -31427,7 +32300,7 @@
       </c>
     </row>
     <row r="15" spans="1:45">
-      <c r="A15" s="33"/>
+      <c r="A15" s="31"/>
       <c r="B15" t="s">
         <v>218</v>
       </c>
@@ -31508,7 +32381,7 @@
       </c>
     </row>
     <row r="16" spans="1:45">
-      <c r="A16" s="33"/>
+      <c r="A16" s="31"/>
       <c r="B16" t="s">
         <v>219</v>
       </c>
@@ -31640,7 +32513,7 @@
       </c>
     </row>
     <row r="17" spans="1:45">
-      <c r="A17" s="33"/>
+      <c r="A17" s="31"/>
       <c r="B17" t="s">
         <v>64</v>
       </c>
@@ -31772,7 +32645,7 @@
       </c>
     </row>
     <row r="18" spans="1:45">
-      <c r="A18" s="33"/>
+      <c r="A18" s="31"/>
       <c r="B18" t="s">
         <v>65</v>
       </c>
@@ -31904,7 +32777,7 @@
       </c>
     </row>
     <row r="19" spans="1:45">
-      <c r="A19" s="33"/>
+      <c r="A19" s="31"/>
       <c r="B19" t="s">
         <v>66</v>
       </c>
@@ -31982,7 +32855,7 @@
       </c>
     </row>
     <row r="20" spans="1:45">
-      <c r="A20" s="33"/>
+      <c r="A20" s="31"/>
       <c r="B20" t="s">
         <v>67</v>
       </c>
@@ -32114,7 +32987,7 @@
       </c>
     </row>
     <row r="21" spans="1:45">
-      <c r="A21" s="33"/>
+      <c r="A21" s="31"/>
       <c r="B21" t="s">
         <v>68</v>
       </c>
@@ -32246,7 +33119,7 @@
       </c>
     </row>
     <row r="22" spans="1:45">
-      <c r="A22" s="33"/>
+      <c r="A22" s="31"/>
       <c r="B22" t="s">
         <v>69</v>
       </c>
@@ -32378,7 +33251,7 @@
       </c>
     </row>
     <row r="23" spans="1:45">
-      <c r="A23" s="33"/>
+      <c r="A23" s="31"/>
       <c r="B23" t="s">
         <v>70</v>
       </c>
@@ -33012,7 +33885,7 @@
       </c>
     </row>
     <row r="29" spans="1:45">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="31" t="s">
         <v>78</v>
       </c>
       <c r="B29" t="s">
@@ -33146,7 +34019,7 @@
       </c>
     </row>
     <row r="30" spans="1:45">
-      <c r="A30" s="33"/>
+      <c r="A30" s="31"/>
       <c r="B30" t="s">
         <v>222</v>
       </c>
@@ -33275,7 +34148,7 @@
       </c>
     </row>
     <row r="31" spans="1:45">
-      <c r="A31" s="33"/>
+      <c r="A31" s="31"/>
       <c r="B31" t="s">
         <v>223</v>
       </c>
@@ -33359,7 +34232,7 @@
       </c>
     </row>
     <row r="32" spans="1:45">
-      <c r="A32" s="33"/>
+      <c r="A32" s="31"/>
       <c r="B32" t="s">
         <v>224</v>
       </c>
@@ -33473,7 +34346,7 @@
       </c>
     </row>
     <row r="33" spans="1:45">
-      <c r="A33" s="33"/>
+      <c r="A33" s="31"/>
       <c r="B33" t="s">
         <v>225</v>
       </c>
@@ -33545,7 +34418,7 @@
       </c>
     </row>
     <row r="34" spans="1:45">
-      <c r="A34" s="33"/>
+      <c r="A34" s="31"/>
       <c r="B34" t="s">
         <v>226</v>
       </c>
@@ -33787,7 +34660,7 @@
       </c>
     </row>
     <row r="36" spans="1:45">
-      <c r="A36" s="33" t="s">
+      <c r="A36" s="31" t="s">
         <v>227</v>
       </c>
       <c r="B36" t="s">
@@ -33912,7 +34785,7 @@
       </c>
     </row>
     <row r="37" spans="1:45">
-      <c r="A37" s="33"/>
+      <c r="A37" s="31"/>
       <c r="B37" t="s">
         <v>229</v>
       </c>
@@ -33999,7 +34872,7 @@
       </c>
     </row>
     <row r="38" spans="1:45">
-      <c r="A38" s="33"/>
+      <c r="A38" s="31"/>
       <c r="B38" t="s">
         <v>230</v>
       </c>
@@ -34077,7 +34950,7 @@
       </c>
     </row>
     <row r="39" spans="1:45">
-      <c r="A39" s="33"/>
+      <c r="A39" s="31"/>
       <c r="B39" t="s">
         <v>227</v>
       </c>
@@ -34173,7 +35046,7 @@
       </c>
     </row>
     <row r="40" spans="1:45">
-      <c r="A40" s="33"/>
+      <c r="A40" s="31"/>
       <c r="B40" t="s">
         <v>231</v>
       </c>
@@ -34388,7 +35261,7 @@
       </c>
     </row>
     <row r="42" spans="1:45">
-      <c r="A42" s="33" t="s">
+      <c r="A42" s="31" t="s">
         <v>232</v>
       </c>
       <c r="B42" t="s">
@@ -34399,7 +35272,7 @@
       </c>
     </row>
     <row r="43" spans="1:45">
-      <c r="A43" s="33"/>
+      <c r="A43" s="31"/>
       <c r="B43" t="s">
         <v>227</v>
       </c>
@@ -34411,7 +35284,7 @@
       </c>
     </row>
     <row r="44" spans="1:45">
-      <c r="A44" s="33"/>
+      <c r="A44" s="31"/>
       <c r="B44" t="s">
         <v>71</v>
       </c>
@@ -34420,7 +35293,7 @@
       </c>
     </row>
     <row r="45" spans="1:45">
-      <c r="A45" s="33"/>
+      <c r="A45" s="31"/>
       <c r="B45" t="s">
         <v>235</v>
       </c>
@@ -34432,13 +35305,13 @@
       </c>
     </row>
     <row r="46" spans="1:45">
-      <c r="A46" s="33"/>
+      <c r="A46" s="31"/>
       <c r="C46" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="47" spans="1:45">
-      <c r="A47" s="33"/>
+      <c r="A47" s="31"/>
       <c r="C47" t="s">
         <v>94</v>
       </c>
@@ -34453,7 +35326,7 @@
       </c>
     </row>
     <row r="48" spans="1:45">
-      <c r="A48" s="33"/>
+      <c r="A48" s="31"/>
       <c r="B48" t="s">
         <v>242</v>
       </c>
@@ -34462,7 +35335,7 @@
       </c>
     </row>
     <row r="49" spans="1:24">
-      <c r="A49" s="33"/>
+      <c r="A49" s="31"/>
       <c r="C49" t="s">
         <v>238</v>
       </c>
@@ -34477,7 +35350,7 @@
       </c>
     </row>
     <row r="50" spans="1:24">
-      <c r="A50" s="33"/>
+      <c r="A50" s="31"/>
       <c r="C50" t="s">
         <v>94</v>
       </c>
@@ -34489,7 +35362,7 @@
       </c>
     </row>
     <row r="51" spans="1:24">
-      <c r="A51" s="33"/>
+      <c r="A51" s="31"/>
       <c r="B51" t="s">
         <v>240</v>
       </c>
@@ -34516,7 +35389,7 @@
       </c>
     </row>
     <row r="52" spans="1:24">
-      <c r="A52" s="33"/>
+      <c r="A52" s="31"/>
       <c r="C52" t="s">
         <v>238</v>
       </c>
@@ -34540,7 +35413,7 @@
       </c>
     </row>
     <row r="53" spans="1:24">
-      <c r="A53" s="33"/>
+      <c r="A53" s="31"/>
       <c r="C53" t="s">
         <v>94</v>
       </c>
@@ -34617,7 +35490,7 @@
       </c>
     </row>
     <row r="55" spans="1:24">
-      <c r="A55" s="33" t="s">
+      <c r="A55" s="31" t="s">
         <v>255</v>
       </c>
       <c r="B55" t="s">
@@ -34637,7 +35510,7 @@
       </c>
     </row>
     <row r="56" spans="1:24">
-      <c r="A56" s="33"/>
+      <c r="A56" s="31"/>
       <c r="C56" t="s">
         <v>208</v>
       </c>
@@ -34649,7 +35522,7 @@
       </c>
     </row>
     <row r="57" spans="1:24">
-      <c r="A57" s="33"/>
+      <c r="A57" s="31"/>
       <c r="C57" t="s">
         <v>207</v>
       </c>
@@ -34667,7 +35540,7 @@
       </c>
     </row>
     <row r="58" spans="1:24">
-      <c r="A58" s="33"/>
+      <c r="A58" s="31"/>
       <c r="C58" t="s">
         <v>209</v>
       </c>
@@ -34676,7 +35549,7 @@
       </c>
     </row>
     <row r="59" spans="1:24">
-      <c r="A59" s="33"/>
+      <c r="A59" s="31"/>
       <c r="C59" t="s">
         <v>256</v>
       </c>
@@ -34697,7 +35570,7 @@
       </c>
     </row>
     <row r="60" spans="1:24">
-      <c r="A60" s="33"/>
+      <c r="A60" s="31"/>
       <c r="C60" t="s">
         <v>94</v>
       </c>
@@ -34718,7 +35591,7 @@
       </c>
     </row>
     <row r="61" spans="1:24">
-      <c r="A61" s="33"/>
+      <c r="A61" s="31"/>
       <c r="B61" t="s">
         <v>212</v>
       </c>
@@ -34742,7 +35615,7 @@
       </c>
     </row>
     <row r="62" spans="1:24">
-      <c r="A62" s="33"/>
+      <c r="A62" s="31"/>
       <c r="C62" t="s">
         <v>69</v>
       </c>
@@ -34754,7 +35627,7 @@
       </c>
     </row>
     <row r="63" spans="1:24">
-      <c r="A63" s="33"/>
+      <c r="A63" s="31"/>
       <c r="C63" t="s">
         <v>94</v>
       </c>
@@ -34763,7 +35636,7 @@
       </c>
     </row>
     <row r="64" spans="1:24">
-      <c r="A64" s="33"/>
+      <c r="A64" s="31"/>
       <c r="B64" t="s">
         <v>78</v>
       </c>
@@ -34772,7 +35645,7 @@
       </c>
     </row>
     <row r="65" spans="1:45">
-      <c r="A65" s="33"/>
+      <c r="A65" s="31"/>
       <c r="B65" t="s">
         <v>74</v>
       </c>
@@ -34781,7 +35654,7 @@
       </c>
     </row>
     <row r="66" spans="1:45">
-      <c r="A66" s="33"/>
+      <c r="A66" s="31"/>
       <c r="B66" t="s">
         <v>71</v>
       </c>
@@ -34790,7 +35663,7 @@
       </c>
     </row>
     <row r="67" spans="1:45">
-      <c r="A67" s="33"/>
+      <c r="A67" s="31"/>
       <c r="B67" t="s">
         <v>227</v>
       </c>
@@ -34802,7 +35675,7 @@
       </c>
     </row>
     <row r="68" spans="1:45">
-      <c r="A68" s="33"/>
+      <c r="A68" s="31"/>
       <c r="B68" t="s">
         <v>231</v>
       </c>
@@ -35696,20 +36569,20 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="Y2:AE2"/>
+    <mergeCell ref="D1:X1"/>
+    <mergeCell ref="Y1:AS1"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A10:A23"/>
+    <mergeCell ref="AF2:AL2"/>
+    <mergeCell ref="AM2:AS2"/>
     <mergeCell ref="A42:A53"/>
     <mergeCell ref="A55:A68"/>
     <mergeCell ref="D2:J2"/>
     <mergeCell ref="K2:Q2"/>
     <mergeCell ref="R2:X2"/>
-    <mergeCell ref="Y2:AE2"/>
-    <mergeCell ref="D1:X1"/>
-    <mergeCell ref="Y1:AS1"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A10:A23"/>
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A36:A40"/>
-    <mergeCell ref="AF2:AL2"/>
-    <mergeCell ref="AM2:AS2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>